<commit_message>
include Debts and Fixed Assets in example HFPs
</commit_message>
<xml_diff>
--- a/examples/joe.xlsx
+++ b/examples/joe.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\Owl\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C3497A-D4CB-44F3-AF48-5204920222DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C51DFC-C539-44DA-B233-010F3A9DFC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21240" yWindow="15780" windowWidth="15045" windowHeight="11700" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Joe" sheetId="1" r:id="rId1"/>
+    <sheet name="Debts" sheetId="2" r:id="rId2"/>
+    <sheet name="Fixed Assets" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>year</t>
   </si>
@@ -63,6 +65,33 @@
   </si>
   <si>
     <t>Roth IRA ctrb</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>basis</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>yod</t>
+  </si>
+  <si>
+    <t>commission</t>
   </si>
 </sst>
 </file>
@@ -72,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +115,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,10 +145,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,28 +468,28 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -479,7 +518,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -494,7 +533,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -509,7 +548,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2022</v>
       </c>
@@ -524,7 +563,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2023</v>
       </c>
@@ -539,7 +578,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2024</v>
       </c>
@@ -554,7 +593,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2025</v>
       </c>
@@ -573,7 +612,7 @@
         <v>-40000</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2026</v>
       </c>
@@ -590,7 +629,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2027</v>
       </c>
@@ -605,7 +644,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2028</v>
       </c>
@@ -618,7 +657,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2029</v>
       </c>
@@ -631,7 +670,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2030</v>
       </c>
@@ -644,7 +683,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2031</v>
       </c>
@@ -657,7 +696,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2032</v>
       </c>
@@ -670,7 +709,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2033</v>
       </c>
@@ -683,7 +722,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2034</v>
       </c>
@@ -696,7 +735,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2035</v>
       </c>
@@ -709,7 +748,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2036</v>
       </c>
@@ -722,7 +761,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2037</v>
       </c>
@@ -735,7 +774,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2038</v>
       </c>
@@ -748,7 +787,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2039</v>
       </c>
@@ -761,7 +800,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2040</v>
       </c>
@@ -774,7 +813,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2041</v>
       </c>
@@ -787,7 +826,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2042</v>
       </c>
@@ -800,7 +839,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2043</v>
       </c>
@@ -813,7 +852,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2044</v>
       </c>
@@ -826,7 +865,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2045</v>
       </c>
@@ -839,7 +878,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2046</v>
       </c>
@@ -852,7 +891,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2047</v>
       </c>
@@ -865,7 +904,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2048</v>
       </c>
@@ -878,7 +917,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2049</v>
       </c>
@@ -891,7 +930,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2050</v>
       </c>
@@ -904,7 +943,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2051</v>
       </c>
@@ -917,7 +956,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2052</v>
       </c>
@@ -930,7 +969,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2053</v>
       </c>
@@ -943,7 +982,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2054</v>
       </c>
@@ -956,9 +995,85 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2055</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3C0449-2F72-4E2B-B58A-DAF3F8341110}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5858D1C-D856-4B47-BFF3-E4813D8F26DA}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="7" width="12.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>